<commit_message>
Primera y segunda entrega (nuevo formato)
</commit_message>
<xml_diff>
--- a/Primera Entrega/Clase 9- Cierre Estructura y Memorias/Memorias.xlsx
+++ b/Primera Entrega/Clase 9- Cierre Estructura y Memorias/Memorias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos\Documents\Marcos\Programación\DigitalHouse\Introducción_a_la_informática\VSC\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos\Documents\Marcos\Programación\DigitalHouse\Introducción_a_la_informática\VSC\Mochila backup\Clase 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Intel</t>
   </si>
@@ -47,18 +47,9 @@
     <t>Core i3 7100</t>
   </si>
   <si>
-    <t>Motherboard Gigabyte H410M-H V3 1200</t>
-  </si>
-  <si>
-    <t>Memoria Ram OEM 4GB 2666 Mhz DDR4 BULK</t>
-  </si>
-  <si>
     <t>Disco Solido SSD 120GB Adata SU650 Ultimate SATA III</t>
   </si>
   <si>
-    <t>Motherboard Asus Prime A520m-k</t>
-  </si>
-  <si>
     <t>Ryzen 3 2200g</t>
   </si>
   <si>
@@ -77,15 +68,6 @@
     <t>GeForce GT 1030 2GD4 LP OC</t>
   </si>
   <si>
-    <t>Micro Intel I5-12400 4.4 Ghz 18Mb S.1700</t>
-  </si>
-  <si>
-    <t>Motherboard Asus Prime Z690-P D4 LGA S1700</t>
-  </si>
-  <si>
-    <t>Memoria Ram Kingston Fury Beast RGB 8GB 3200 Mhz DDR4</t>
-  </si>
-  <si>
     <t>Disco Solido SSD 480GB Kingston A400 SATA III</t>
   </si>
   <si>
@@ -107,15 +89,6 @@
     <t>AMD Ryzen 7 3800xt</t>
   </si>
   <si>
-    <t>Motherboard Asrock Z590 OC Formula 1200</t>
-  </si>
-  <si>
-    <t>Memoria Ram Adata Xpg Spectrix D50 RGB 32GB 3200 Mhz DDR4 Grey</t>
-  </si>
-  <si>
-    <t>Placa De Video EVGA RTX 3090 FTW3 ULTRA ICX3 24GB GDDR6X ARGB</t>
-  </si>
-  <si>
     <t>Disco Solido SSD 2TB Adata SwordFish M.2 NVMe PCIe X4 3.0</t>
   </si>
   <si>
@@ -125,13 +98,43 @@
     <t>Disco Solido SSD 2TB Adata SwordFish M.2 NVMe PCIe X4 3.2</t>
   </si>
   <si>
-    <t>Motherboard Asrock X570 Steel Legend AM4</t>
-  </si>
-  <si>
-    <t>Motherboard Asrock X570 Steel Legend AM3</t>
-  </si>
-  <si>
-    <t>Memoria Ram OLOY WarHawk Black RGB 32GB 3000 Mhz DDR4</t>
+    <t>Asus H170-PLUS D3</t>
+  </si>
+  <si>
+    <t>Kingston KVR16N11H/4 4 GB</t>
+  </si>
+  <si>
+    <t>MSI A320M-A PRO</t>
+  </si>
+  <si>
+    <t>Corsair Vengeance LPX 4 GB</t>
+  </si>
+  <si>
+    <t>Gigabyte Z690 AERO G ATX LGA1700 Motherboard</t>
+  </si>
+  <si>
+    <t>Intel Core i5-12600K 3.7 GHz 10-Core Processor</t>
+  </si>
+  <si>
+    <t>Kingston FURY Beast 32 GB</t>
+  </si>
+  <si>
+    <t>Gigabyte Z490 AORUS XTREME</t>
+  </si>
+  <si>
+    <t>Corsair Vengeance RGB Pro 64 GB</t>
+  </si>
+  <si>
+    <t>Sapphire 11256-00</t>
+  </si>
+  <si>
+    <t>ASRock X470 Taichi</t>
+  </si>
+  <si>
+    <t>Sapphire 11256-01</t>
+  </si>
+  <si>
+    <t>Sapphire 11256-02</t>
   </si>
 </sst>
 </file>
@@ -589,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +605,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -611,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,38 +625,38 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -661,19 +664,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -682,21 +685,21 @@
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -704,27 +707,27 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -732,33 +735,33 @@
         <v>5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>0</v>
@@ -767,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,41 +778,41 @@
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -817,27 +820,27 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>